<commit_message>
m2 & b updated
</commit_message>
<xml_diff>
--- a/B-pojat.xlsx
+++ b/B-pojat.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\own_prog\github\kaudet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48CE78DB-65D5-4269-B024-568BCC5372EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{679CC270-6D1D-40FC-AD22-64889F956F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="192" windowWidth="20604" windowHeight="13200" tabRatio="880" activeTab="1" xr2:uid="{CFC6D258-5D3C-46F8-BFEC-F3C271445404}"/>
+    <workbookView xWindow="1092" yWindow="948" windowWidth="20880" windowHeight="12012" tabRatio="880" activeTab="1" xr2:uid="{CFC6D258-5D3C-46F8-BFEC-F3C271445404}"/>
   </bookViews>
   <sheets>
     <sheet name="B 2023-2026" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="126">
   <si>
     <t>päivä</t>
   </si>
@@ -405,6 +405,18 @@
   </si>
   <si>
     <t>21-25,21-25</t>
+  </si>
+  <si>
+    <t>23-25,25-19,25-17</t>
+  </si>
+  <si>
+    <t>OsVa2</t>
+  </si>
+  <si>
+    <t>25-19,15-25,0-25</t>
+  </si>
+  <si>
+    <t>A-V</t>
   </si>
 </sst>
 </file>
@@ -498,7 +510,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -546,6 +558,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1005,36 +1020,36 @@
         <v>111</v>
       </c>
       <c r="C4" s="11">
+        <f>'B 2025-2026'!R2</f>
+        <v>7</v>
+      </c>
+      <c r="D4" s="11">
+        <f>'B 2025-2026'!O2</f>
+        <v>4</v>
+      </c>
+      <c r="E4" s="11">
+        <f>'B 2025-2026'!P4</f>
+        <v>0</v>
+      </c>
+      <c r="F4" s="11">
         <f>'B 2025-2026'!Q2</f>
-        <v>6</v>
-      </c>
-      <c r="D4" s="11">
-        <f>'B 2025-2026'!N2</f>
         <v>3</v>
       </c>
-      <c r="E4" s="11">
+      <c r="G4" s="11">
+        <f>'B 2025-2026'!O3</f>
+        <v>9</v>
+      </c>
+      <c r="H4" s="11">
+        <f>'B 2025-2026'!Q5</f>
+        <v>0</v>
+      </c>
+      <c r="I4" s="11">
         <f>'B 2025-2026'!O4</f>
-        <v>0</v>
-      </c>
-      <c r="F4" s="11">
-        <f>'B 2025-2026'!P2</f>
-        <v>3</v>
-      </c>
-      <c r="G4" s="11">
-        <f>'B 2025-2026'!N3</f>
-        <v>6</v>
-      </c>
-      <c r="H4" s="11">
-        <f>'B 2025-2026'!P5</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="11">
-        <f>'B 2025-2026'!N4</f>
-        <v>298</v>
+        <v>411</v>
       </c>
       <c r="J4" s="11">
-        <f>'B 2025-2026'!P4</f>
-        <v>247</v>
+        <f>'B 2025-2026'!Q4</f>
+        <v>377</v>
       </c>
       <c r="K4" s="11"/>
     </row>
@@ -1045,11 +1060,11 @@
       </c>
       <c r="C5" s="7">
         <f t="shared" ref="C5:J5" si="0">SUM(C2:C4)</f>
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
@@ -1061,7 +1076,7 @@
       </c>
       <c r="G5" s="9">
         <f t="shared" si="0"/>
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="H5" s="9">
         <f t="shared" si="0"/>
@@ -1069,11 +1084,11 @@
       </c>
       <c r="I5" s="9">
         <f t="shared" si="0"/>
-        <v>2612</v>
+        <v>2725</v>
       </c>
       <c r="J5" s="9">
         <f t="shared" si="0"/>
-        <v>2605</v>
+        <v>2735</v>
       </c>
       <c r="K5" s="8"/>
     </row>
@@ -1088,18 +1103,18 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="18" width="10.77734375" customWidth="1"/>
+    <col min="1" max="19" width="10.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -1115,39 +1130,42 @@
         <v>3</v>
       </c>
       <c r="G1" s="18">
+        <v>3</v>
+      </c>
+      <c r="H1" s="18">
         <v>2</v>
       </c>
-      <c r="H1" s="18">
-        <v>1</v>
-      </c>
       <c r="I1" s="18">
+        <v>1</v>
+      </c>
+      <c r="J1" s="18">
         <v>0</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>4</v>
       </c>
       <c r="K1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="18"/>
+      <c r="L1" s="18" t="s">
+        <v>4</v>
+      </c>
       <c r="M1" s="18"/>
-      <c r="N1" s="18" t="s">
-        <v>81</v>
-      </c>
+      <c r="N1" s="18"/>
       <c r="O1" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="P1" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="18" t="s">
+      <c r="Q1" s="18" t="s">
         <v>5</v>
-      </c>
-      <c r="Q1" s="18" t="s">
-        <v>6</v>
       </c>
       <c r="R1" s="18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S1" s="18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="15">
         <v>45934</v>
       </c>
@@ -1166,40 +1184,41 @@
       <c r="F2" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="G2" s="16">
-        <v>1</v>
-      </c>
-      <c r="H2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16">
+        <v>1</v>
+      </c>
       <c r="I2" s="16"/>
-      <c r="J2" s="16">
+      <c r="J2" s="16"/>
+      <c r="K2" s="16">
         <v>50</v>
       </c>
-      <c r="K2" s="16">
+      <c r="L2" s="16">
         <v>17</v>
       </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="16"/>
+      <c r="N2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="N2" s="16">
-        <f>SUM(G2:G24)</f>
+      <c r="O2" s="16">
+        <f>SUM(H2:H24)</f>
+        <v>4</v>
+      </c>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16">
+        <f>SUM(J2:J24)</f>
         <v>3</v>
       </c>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16">
-        <f>SUM(I2:I24)</f>
-        <v>3</v>
-      </c>
-      <c r="Q2" s="16">
-        <f>SUM(N2:P2)</f>
-        <v>6</v>
-      </c>
       <c r="R2" s="16">
-        <f>Q2*2</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+        <f>SUM(O2:Q2)</f>
+        <v>7</v>
+      </c>
+      <c r="S2" s="16">
+        <f>R2*2</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A3" s="22">
         <v>45934</v>
       </c>
@@ -1218,37 +1237,38 @@
       <c r="F3" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="G3" s="13">
-        <v>1</v>
-      </c>
-      <c r="H3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="13">
+        <v>1</v>
+      </c>
       <c r="I3" s="13"/>
-      <c r="J3" s="13">
+      <c r="J3" s="13"/>
+      <c r="K3" s="13">
         <v>50</v>
       </c>
-      <c r="K3" s="13">
+      <c r="L3" s="13">
         <v>22</v>
       </c>
-      <c r="L3" s="13"/>
-      <c r="M3" s="20" t="s">
+      <c r="M3" s="13"/>
+      <c r="N3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="13">
-        <f>SUM(G2:G24)*2</f>
-        <v>6</v>
-      </c>
-      <c r="O3" s="13"/>
-      <c r="P3" s="13">
-        <f>SUM(I2:I24)*2</f>
-        <v>6</v>
-      </c>
+      <c r="O3" s="13">
+        <f>SUM(H2:H24)*2+SUM(I2:I24)</f>
+        <v>9</v>
+      </c>
+      <c r="P3" s="13"/>
       <c r="Q3" s="13">
-        <f>SUM(N3:P3)</f>
-        <v>12</v>
-      </c>
-      <c r="R3" s="13"/>
-    </row>
-    <row r="4" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+        <f>SUM(J2:J8)*2+2*SUM(I2:I24)+H8</f>
+        <v>9</v>
+      </c>
+      <c r="R3" s="13">
+        <f>SUM(O3:Q3)</f>
+        <v>18</v>
+      </c>
+      <c r="S3" s="13"/>
+    </row>
+    <row r="4" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="15">
         <v>45934</v>
       </c>
@@ -1269,35 +1289,36 @@
       </c>
       <c r="G4" s="16"/>
       <c r="H4" s="16"/>
-      <c r="I4" s="16">
-        <v>1</v>
-      </c>
+      <c r="I4" s="16"/>
       <c r="J4" s="16">
+        <v>1</v>
+      </c>
+      <c r="K4" s="16">
         <v>56</v>
       </c>
-      <c r="K4" s="16">
+      <c r="L4" s="16">
         <v>63</v>
       </c>
-      <c r="L4" s="16"/>
-      <c r="M4" s="19" t="s">
+      <c r="M4" s="16"/>
+      <c r="N4" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="N4" s="16">
-        <f>SUM(J2:J24)</f>
-        <v>298</v>
-      </c>
-      <c r="O4" s="16"/>
-      <c r="P4" s="16">
+      <c r="O4" s="16">
         <f>SUM(K2:K24)</f>
-        <v>247</v>
-      </c>
+        <v>411</v>
+      </c>
+      <c r="P4" s="16"/>
       <c r="Q4" s="16">
-        <f>SUM(N4:P4)</f>
-        <v>545</v>
-      </c>
-      <c r="R4" s="16"/>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+        <f>SUM(L2:L24)</f>
+        <v>377</v>
+      </c>
+      <c r="R4" s="16">
+        <f>SUM(O4:Q4)</f>
+        <v>788</v>
+      </c>
+      <c r="S4" s="16"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>45955</v>
       </c>
@@ -1316,26 +1337,27 @@
       <c r="F5" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="G5" s="13">
-        <v>1</v>
-      </c>
-      <c r="H5" s="13"/>
+      <c r="G5" s="13"/>
+      <c r="H5" s="13">
+        <v>1</v>
+      </c>
       <c r="I5" s="13"/>
-      <c r="J5" s="13">
+      <c r="J5" s="13"/>
+      <c r="K5" s="13">
         <v>50</v>
       </c>
-      <c r="K5" s="13">
+      <c r="L5" s="13">
         <v>34</v>
       </c>
-      <c r="L5" s="13"/>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
       <c r="O5" s="13"/>
       <c r="P5" s="13"/>
       <c r="Q5" s="13"/>
       <c r="R5" s="13"/>
-    </row>
-    <row r="6" spans="1:18" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="S5" s="13"/>
+    </row>
+    <row r="6" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>46320</v>
       </c>
@@ -1356,24 +1378,25 @@
       </c>
       <c r="G6" s="16"/>
       <c r="H6" s="16"/>
-      <c r="I6" s="16">
-        <v>1</v>
-      </c>
+      <c r="I6" s="16"/>
       <c r="J6" s="16">
+        <v>1</v>
+      </c>
+      <c r="K6" s="16">
         <v>50</v>
       </c>
-      <c r="K6" s="16">
+      <c r="L6" s="16">
         <v>61</v>
       </c>
-      <c r="L6" s="16"/>
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
       <c r="O6" s="16"/>
       <c r="P6" s="16"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S6" s="16"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>45955</v>
       </c>
@@ -1394,64 +1417,103 @@
       </c>
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
-      <c r="I7" s="13">
-        <v>1</v>
-      </c>
+      <c r="I7" s="13"/>
       <c r="J7" s="13">
+        <v>1</v>
+      </c>
+      <c r="K7" s="13">
         <v>42</v>
       </c>
-      <c r="K7" s="13">
+      <c r="L7" s="13">
         <v>50</v>
       </c>
-      <c r="L7" s="13"/>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
       <c r="O7" s="13"/>
       <c r="P7" s="13"/>
       <c r="Q7" s="13"/>
       <c r="R7" s="13"/>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A8" s="15"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
+      <c r="S7" s="13"/>
+    </row>
+    <row r="8" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
+        <v>45976</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>122</v>
+      </c>
       <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
+      <c r="H8" s="16">
+        <v>1</v>
+      </c>
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
+      <c r="K8" s="16">
+        <v>73</v>
+      </c>
+      <c r="L8" s="16">
+        <v>61</v>
+      </c>
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
       <c r="O8" s="16"/>
       <c r="P8" s="16"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A9" s="12"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="14"/>
-      <c r="F9" s="13"/>
+      <c r="S8" s="16"/>
+    </row>
+    <row r="9" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="22">
+        <v>45976</v>
+      </c>
+      <c r="B9" s="23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>124</v>
+      </c>
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
-      <c r="I9" s="13"/>
+      <c r="I9" s="13">
+        <v>1</v>
+      </c>
       <c r="J9" s="13"/>
-      <c r="K9" s="13"/>
-      <c r="L9" s="13"/>
+      <c r="K9" s="13">
+        <v>40</v>
+      </c>
+      <c r="L9" s="13">
+        <v>69</v>
+      </c>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
       <c r="O9" s="13"/>
       <c r="P9" s="13"/>
       <c r="Q9" s="13"/>
       <c r="R9" s="13"/>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S9" s="13"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="15"/>
       <c r="B10" s="16"/>
       <c r="C10" s="16"/>
@@ -1470,8 +1532,9 @@
       <c r="P10" s="16"/>
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S10" s="16"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A11" s="12"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -1490,8 +1553,9 @@
       <c r="P11" s="13"/>
       <c r="Q11" s="13"/>
       <c r="R11" s="13"/>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S11" s="13"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A12" s="15"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -1510,8 +1574,9 @@
       <c r="P12" s="16"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S12" s="16"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A13" s="12"/>
       <c r="B13" s="13"/>
       <c r="C13" s="13"/>
@@ -1530,8 +1595,9 @@
       <c r="P13" s="13"/>
       <c r="Q13" s="13"/>
       <c r="R13" s="13"/>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S13" s="13"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A14" s="15"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -1550,8 +1616,9 @@
       <c r="P14" s="16"/>
       <c r="Q14" s="16"/>
       <c r="R14" s="16"/>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S14" s="16"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A15" s="12"/>
       <c r="B15" s="13"/>
       <c r="C15" s="13"/>
@@ -1570,8 +1637,9 @@
       <c r="P15" s="13"/>
       <c r="Q15" s="13"/>
       <c r="R15" s="13"/>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S15" s="13"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A16" s="15"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -1590,8 +1658,9 @@
       <c r="P16" s="16"/>
       <c r="Q16" s="16"/>
       <c r="R16" s="16"/>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S16" s="16"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A17" s="12"/>
       <c r="B17" s="13"/>
       <c r="C17" s="13"/>
@@ -1610,8 +1679,9 @@
       <c r="P17" s="13"/>
       <c r="Q17" s="13"/>
       <c r="R17" s="13"/>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S17" s="13"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A18" s="15"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -1630,8 +1700,9 @@
       <c r="P18" s="16"/>
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S18" s="16"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A19" s="12"/>
       <c r="B19" s="13"/>
       <c r="C19" s="13"/>
@@ -1650,8 +1721,9 @@
       <c r="P19" s="13"/>
       <c r="Q19" s="13"/>
       <c r="R19" s="13"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S19" s="13"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -1670,8 +1742,9 @@
       <c r="P20" s="16"/>
       <c r="Q20" s="16"/>
       <c r="R20" s="16"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S20" s="16"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A21" s="12"/>
       <c r="B21" s="13"/>
       <c r="C21" s="13"/>
@@ -1690,8 +1763,9 @@
       <c r="P21" s="13"/>
       <c r="Q21" s="13"/>
       <c r="R21" s="13"/>
-    </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S21" s="13"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A22" s="15"/>
       <c r="B22" s="16"/>
       <c r="C22" s="16"/>
@@ -1710,8 +1784,9 @@
       <c r="P22" s="16"/>
       <c r="Q22" s="16"/>
       <c r="R22" s="16"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S22" s="16"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A23" s="12"/>
       <c r="B23" s="13"/>
       <c r="C23" s="13"/>
@@ -1730,8 +1805,9 @@
       <c r="P23" s="13"/>
       <c r="Q23" s="13"/>
       <c r="R23" s="13"/>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S23" s="13"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A24" s="15"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -1750,6 +1826,7 @@
       <c r="P24" s="16"/>
       <c r="Q24" s="16"/>
       <c r="R24" s="16"/>
+      <c r="S24" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>